<commit_message>
change stm32f benchmark graphs
</commit_message>
<xml_diff>
--- a/graphs/STM32F/FFT/fft.xlsx
+++ b/graphs/STM32F/FFT/fft.xlsx
@@ -6,8 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FFT_data_CCM" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FFT_data_RAM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FFT_data_CCM code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FFT_data_CCM code_CCM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FFT_data_RAM code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FFT_data_RAM code_CCM" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,32 +464,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>FLASH 24</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CCM 24</t>
+          <t>48</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>FLASH 48</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CCM 48</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>FLASH 72</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>CCM 72</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -501,19 +488,10 @@
         <v>13013.90606424083</v>
       </c>
       <c r="C2" t="n">
-        <v>11699.34893579034</v>
+        <v>22324.88153016039</v>
       </c>
       <c r="D2" t="n">
-        <v>22324.88153016039</v>
-      </c>
-      <c r="E2" t="n">
-        <v>21647.64702320099</v>
-      </c>
-      <c r="F2" t="n">
         <v>28915.4166946868</v>
-      </c>
-      <c r="G2" t="n">
-        <v>29612.40397940437</v>
       </c>
     </row>
     <row r="3">
@@ -526,19 +504,10 @@
         <v>0.0069</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00722</v>
+        <v>0.00406</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00406</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.00384</v>
-      </c>
-      <c r="F3" t="n">
         <v>0.00334</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.00278</v>
       </c>
     </row>
     <row r="4">
@@ -554,28 +523,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(2020.84, 2028.06)</t>
+          <t>(3003.68, 3007.74)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(3003.68, 3007.74)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(3203.0, 3206.84)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>(4182.68, 4186.02)</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>(4381.4, 4384.18)</t>
-        </is>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>296.3266410827637</v>
+      </c>
+      <c r="C5" t="n">
+        <v>299.1087627410889</v>
+      </c>
+      <c r="D5" t="n">
+        <v>318.7057228088379</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -600,32 +570,17 @@
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>FLASH 24</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>CCM 24</t>
+          <t>48</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>FLASH 48</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>CCM 48</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>FLASH 72</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>CCM 72</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -636,22 +591,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13295.41634656712</v>
+        <v>11699.34893579034</v>
       </c>
       <c r="C2" t="n">
-        <v>11903.81436734586</v>
+        <v>21647.64702320099</v>
       </c>
       <c r="D2" t="n">
-        <v>22548.68040279466</v>
-      </c>
-      <c r="E2" t="n">
-        <v>21678.90848738424</v>
-      </c>
-      <c r="F2" t="n">
-        <v>28977.92721387022</v>
-      </c>
-      <c r="G2" t="n">
-        <v>29684.61811542511</v>
+        <v>29612.40397940437</v>
       </c>
     </row>
     <row r="3">
@@ -661,22 +607,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00668</v>
+        <v>0.00722</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00666</v>
+        <v>0.00384</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00392</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.00356</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00322</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.00256</v>
+        <v>0.00278</v>
       </c>
     </row>
     <row r="4">
@@ -687,33 +624,246 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>(2020.84, 2028.06)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(3203.0, 3206.84)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(4381.4, 4384.18)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>278.7486877441406</v>
+      </c>
+      <c r="C5" t="n">
+        <v>274.3189830780029</v>
+      </c>
+      <c r="D5" t="n">
+        <v>271.6641941070557</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>intensity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>13295.41634656712</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22548.68040279466</v>
+      </c>
+      <c r="D2" t="n">
+        <v>28977.92721387022</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>runtime</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.00668</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.00392</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00322</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>(2437.92, 2444.6)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>(3621.88, 3625.8)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(4800.5, 4803.72)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>293.0841579437256</v>
+      </c>
+      <c r="C5" t="n">
+        <v>291.6897296905518</v>
+      </c>
+      <c r="D5" t="n">
+        <v>307.919454574585</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>intensity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11903.81436734586</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21678.90848738424</v>
+      </c>
+      <c r="D2" t="n">
+        <v>29684.61811542511</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>runtime</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.00666</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.00356</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00256</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>(2639.84, 2646.5)</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(3821.16, 3824.72)</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(3621.88, 3625.8)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(3821.16, 3824.72)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(4800.5, 4803.72)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>(4998.98, 5001.54)</t>
         </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>261.6220321655273</v>
+      </c>
+      <c r="C5" t="n">
+        <v>254.68381690979</v>
+      </c>
+      <c r="D5" t="n">
+        <v>250.7756538391114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create compare tab begining
</commit_message>
<xml_diff>
--- a/graphs/STM32F/FFT/fft.xlsx
+++ b/graphs/STM32F/FFT/fft.xlsx
@@ -6,10 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FFT_data_CCM code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FFT_data_CCM code_CCM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="FFT_data_RAM code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="FFT_data_RAM code_CCM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="data_CCM code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="data_CCM code_CCM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="data_RAM code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="data_RAM code_CCM" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13013.90606424083</v>
+        <v>13014</v>
       </c>
       <c r="C2" t="n">
-        <v>22324.88153016039</v>
+        <v>22325</v>
       </c>
       <c r="D2" t="n">
-        <v>28915.4166946868</v>
+        <v>28915</v>
       </c>
     </row>
     <row r="3">
@@ -539,13 +539,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>296.3266410827637</v>
+        <v>0.296</v>
       </c>
       <c r="C5" t="n">
-        <v>299.1087627410889</v>
+        <v>0.299</v>
       </c>
       <c r="D5" t="n">
-        <v>318.7057228088379</v>
+        <v>0.319</v>
       </c>
     </row>
   </sheetData>
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11699.34893579034</v>
+        <v>11699</v>
       </c>
       <c r="C2" t="n">
-        <v>21647.64702320099</v>
+        <v>21648</v>
       </c>
       <c r="D2" t="n">
-        <v>29612.40397940437</v>
+        <v>29612</v>
       </c>
     </row>
     <row r="3">
@@ -645,13 +645,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>278.7486877441406</v>
+        <v>0.279</v>
       </c>
       <c r="C5" t="n">
-        <v>274.3189830780029</v>
+        <v>0.274</v>
       </c>
       <c r="D5" t="n">
-        <v>271.6641941070557</v>
+        <v>0.272</v>
       </c>
     </row>
   </sheetData>
@@ -697,13 +697,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13295.41634656712</v>
+        <v>13295</v>
       </c>
       <c r="C2" t="n">
-        <v>22548.68040279466</v>
+        <v>22549</v>
       </c>
       <c r="D2" t="n">
-        <v>28977.92721387022</v>
+        <v>28978</v>
       </c>
     </row>
     <row r="3">
@@ -751,13 +751,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>293.0841579437256</v>
+        <v>0.293</v>
       </c>
       <c r="C5" t="n">
-        <v>291.6897296905518</v>
+        <v>0.292</v>
       </c>
       <c r="D5" t="n">
-        <v>307.919454574585</v>
+        <v>0.308</v>
       </c>
     </row>
   </sheetData>
@@ -803,13 +803,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11903.81436734586</v>
+        <v>11904</v>
       </c>
       <c r="C2" t="n">
-        <v>21678.90848738424</v>
+        <v>21679</v>
       </c>
       <c r="D2" t="n">
-        <v>29684.61811542511</v>
+        <v>29685</v>
       </c>
     </row>
     <row r="3">
@@ -857,13 +857,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>261.6220321655273</v>
+        <v>0.262</v>
       </c>
       <c r="C5" t="n">
-        <v>254.68381690979</v>
+        <v>0.255</v>
       </c>
       <c r="D5" t="n">
-        <v>250.7756538391114</v>
+        <v>0.251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automatic generation of csv files used for the plot in the latex
</commit_message>
<xml_diff>
--- a/graphs/STM32F/FFT/fft.xlsx
+++ b/graphs/STM32F/FFT/fft.xlsx
@@ -6,10 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data_CCM code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="data_CCM code_CCM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="data_RAM code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="data_RAM code_CCM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="data_CCM-code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="data_CCM-code_CCM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="data_RAM-code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="data_RAM-code_CCM" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>